<commit_message>
First commit of cutie-labels
</commit_message>
<xml_diff>
--- a/disabled products/Gen 2.5 Elliptical Cooler.xlsx
+++ b/disabled products/Gen 2.5 Elliptical Cooler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrypkahauer/Developer/Python/Jenn/prod_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenn/Documents/QuikTrip/2024 Reset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DC1C7D-D30C-DC4E-918A-5B629AEAF553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AB38CA-A0FD-9F45-9B9A-4AB043B9B8CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{4014FEC5-9A1E-F046-88FD-58136A531ECB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12680" windowHeight="14400" xr2:uid="{4014FEC5-9A1E-F046-88FD-58136A531ECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="240">
   <si>
     <t>040822011907</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Red Pepper Hummus w/Pretzels</t>
   </si>
   <si>
-    <t>044529147815</t>
-  </si>
-  <si>
-    <t>Snackups Cheddar and Pretzel</t>
-  </si>
-  <si>
     <t>810051010107</t>
   </si>
   <si>
@@ -381,12 +375,6 @@
     <t>Van Holte Hot Pickle</t>
   </si>
   <si>
-    <t>027541000054</t>
-  </si>
-  <si>
-    <t>Niagra .5L</t>
-  </si>
-  <si>
     <t>049000177855</t>
   </si>
   <si>
@@ -405,12 +393,6 @@
     <t>Coke Spiced 12oz Can Slim</t>
   </si>
   <si>
-    <t>049000555370</t>
-  </si>
-  <si>
-    <t>Coke Spiced Zero 12oz Can Slim</t>
-  </si>
-  <si>
     <t>049000177824</t>
   </si>
   <si>
@@ -489,24 +471,12 @@
     <t>Chobani Cookies &amp; Cream 10oz</t>
   </si>
   <si>
-    <t>044700101841</t>
-  </si>
-  <si>
-    <t>OM Natural Plate Salami</t>
-  </si>
-  <si>
     <t>044700101827</t>
   </si>
   <si>
     <t>OM Natural Plate Turkey</t>
   </si>
   <si>
-    <t>044700101797</t>
-  </si>
-  <si>
-    <t>OM Natural Plate Ham</t>
-  </si>
-  <si>
     <t>044500201823</t>
   </si>
   <si>
@@ -621,24 +591,12 @@
     <t>JL Cold Craft Beef Cheddar 3oz</t>
   </si>
   <si>
-    <t>044700074282</t>
-  </si>
-  <si>
-    <t>P3 Red Chicken/Jack/Cashew</t>
-  </si>
-  <si>
     <t>044700070758</t>
   </si>
   <si>
     <t>P3 Green Turkey/Colby/Almond</t>
   </si>
   <si>
-    <t>044700074275</t>
-  </si>
-  <si>
-    <t>P3 Blue Ham/Colby/Cashew</t>
-  </si>
-  <si>
     <t>044700075293</t>
   </si>
   <si>
@@ -696,6 +654,9 @@
     <t>852311004273</t>
   </si>
   <si>
+    <t>Bai Moiokai Coconut</t>
+  </si>
+  <si>
     <t>898999010229</t>
   </si>
   <si>
@@ -732,7 +693,58 @@
     <t>Fiji Water 500mL</t>
   </si>
   <si>
-    <t>Bai Molokai Coconut</t>
+    <t>695119600311</t>
+  </si>
+  <si>
+    <t>Pork Potsticker</t>
+  </si>
+  <si>
+    <t>632432000558</t>
+  </si>
+  <si>
+    <t>Guayaki Yerba Mate Revel Berry 11.5oz</t>
+  </si>
+  <si>
+    <t>632432000510</t>
+  </si>
+  <si>
+    <t>Guayaki Yerba Mate Enlighten Mint 11.5oz</t>
+  </si>
+  <si>
+    <t>632432000480</t>
+  </si>
+  <si>
+    <t>Guayaki Yerba Mate Bluephoria 11.5oz</t>
+  </si>
+  <si>
+    <t>632432000534</t>
+  </si>
+  <si>
+    <t>Guayaki Yerba Mate Peach Revival 11.5oz</t>
+  </si>
+  <si>
+    <t>049000555820</t>
+  </si>
+  <si>
+    <t>Sprite Chill 12oz Can Slim</t>
+  </si>
+  <si>
+    <t>037600183901</t>
+  </si>
+  <si>
+    <t>Hormel Gatherings Tray Pepperoni</t>
+  </si>
+  <si>
+    <t>046100353608</t>
+  </si>
+  <si>
+    <t>Wheat Thins Balance Break</t>
+  </si>
+  <si>
+    <t>046100354063</t>
+  </si>
+  <si>
+    <t>Ritz Balance Break</t>
   </si>
 </sst>
 </file>
@@ -789,9 +801,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -829,7 +841,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -935,7 +947,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,7 +1089,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1085,22 +1097,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F37C57-903E-A843-AA98-99B93DCDCF13}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1111,7 +1123,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1122,7 +1134,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1144,7 +1156,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1199,7 +1211,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
@@ -1243,13 +1255,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1257,10 +1269,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1268,10 +1280,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1279,10 +1291,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1290,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1301,10 +1313,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1312,10 +1324,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1323,10 +1335,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1334,10 +1346,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1345,10 +1357,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1356,10 +1368,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1367,10 +1379,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1378,10 +1390,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1389,10 +1401,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1400,10 +1412,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1411,10 +1423,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1422,10 +1434,10 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1433,10 +1445,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1444,10 +1456,10 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1455,10 +1467,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1466,10 +1478,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1477,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1488,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1499,10 +1511,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1510,10 +1522,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1521,10 +1533,10 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1532,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1543,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1554,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1565,10 +1577,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1576,10 +1588,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1587,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1598,10 +1610,10 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,10 +1621,10 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1620,10 +1632,10 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1631,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1642,10 +1654,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1653,10 +1665,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1664,10 +1676,10 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1675,10 +1687,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1686,10 +1698,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1697,10 +1709,10 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1708,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1719,10 +1731,10 @@
         <v>1</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1730,10 +1742,10 @@
         <v>2</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1741,21 +1753,21 @@
         <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>224</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1763,10 +1775,10 @@
         <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>120</v>
+        <v>226</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1774,43 +1786,43 @@
         <v>2</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>228</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1818,43 +1830,43 @@
         <v>1</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>232</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1862,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1873,21 +1885,21 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1895,21 +1907,21 @@
         <v>2</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1917,21 +1929,21 @@
         <v>1</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1939,10 +1951,10 @@
         <v>1</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,10 +1962,10 @@
         <v>1</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1961,10 +1973,10 @@
         <v>1</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1972,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1983,10 +1995,10 @@
         <v>1</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>160</v>
+        <v>234</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1994,10 +2006,10 @@
         <v>1</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2005,10 +2017,10 @@
         <v>1</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2016,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2027,10 +2039,10 @@
         <v>1</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C85" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2038,32 +2050,32 @@
         <v>1</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C86" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C87" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C88" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2071,10 +2083,10 @@
         <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C89" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2082,32 +2094,32 @@
         <v>2</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C90" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2115,10 +2127,10 @@
         <v>1</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2126,10 +2138,10 @@
         <v>1</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2137,10 +2149,10 @@
         <v>1</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C95" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2148,10 +2160,10 @@
         <v>1</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C96" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2159,10 +2171,10 @@
         <v>1</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C97" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2170,10 +2182,10 @@
         <v>1</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2181,21 +2193,21 @@
         <v>1</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2203,10 +2215,10 @@
         <v>1</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2214,10 +2226,10 @@
         <v>1</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2225,21 +2237,21 @@
         <v>1</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="C104" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2247,109 +2259,109 @@
         <v>1</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C107" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C108" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="C112" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C114" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2357,10 +2369,10 @@
         <v>1</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2368,43 +2380,65 @@
         <v>1</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C116" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="C117" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>60</v>
+        <v>216</v>
       </c>
       <c r="C118" t="s">
-        <v>61</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C119" t="s">
-        <v>234</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>5</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C121" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>